<commit_message>
add new dialog message for generation of excel file
</commit_message>
<xml_diff>
--- a/lecturas_sensores.xlsx
+++ b/lecturas_sensores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1415,6 +1415,230 @@
         <v>138</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:27:00 2024</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>128</v>
+      </c>
+      <c r="D62" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:27:00 2024</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>128</v>
+      </c>
+      <c r="D63" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:27:01 2024</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>128</v>
+      </c>
+      <c r="D64" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:27:11 2024</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>127</v>
+      </c>
+      <c r="D65" t="n">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:27:21 2024</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>127</v>
+      </c>
+      <c r="D66" t="n">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:27:31 2024</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>127</v>
+      </c>
+      <c r="D67" t="n">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:27:41 2024</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>126</v>
+      </c>
+      <c r="D68" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:27:51 2024</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>126</v>
+      </c>
+      <c r="D69" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:28:01 2024</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>126</v>
+      </c>
+      <c r="D70" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:28:11 2024</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>126</v>
+      </c>
+      <c r="D71" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:37:01 2024</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>147</v>
+      </c>
+      <c r="D72" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:37:01 2024</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>149</v>
+      </c>
+      <c r="D73" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:37:01 2024</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>153</v>
+      </c>
+      <c r="D74" t="n">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 00:37:09 2024</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>150</v>
+      </c>
+      <c r="D75" t="n">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
clean code  in main.ino
</commit_message>
<xml_diff>
--- a/lecturas_sensores.xlsx
+++ b/lecturas_sensores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D135"/>
+  <dimension ref="A1:D358"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2599,6 +2599,3574 @@
         <v>130</v>
       </c>
     </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>135</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:23:50 2024</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>123</v>
+      </c>
+      <c r="D136" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>136</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:24:00 2024</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>123</v>
+      </c>
+      <c r="D137" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>137</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:24:10 2024</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>123</v>
+      </c>
+      <c r="D138" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>138</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:24:20 2024</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>123</v>
+      </c>
+      <c r="D139" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>139</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:24:30 2024</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>123</v>
+      </c>
+      <c r="D140" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>140</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:24:40 2024</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>122</v>
+      </c>
+      <c r="D141" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>141</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:24:50 2024</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>121</v>
+      </c>
+      <c r="D142" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>142</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:25:00 2024</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>120</v>
+      </c>
+      <c r="D143" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>143</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:25:10 2024</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>120</v>
+      </c>
+      <c r="D144" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>144</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:25:20 2024</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>120</v>
+      </c>
+      <c r="D145" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:25:30 2024</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>120</v>
+      </c>
+      <c r="D146" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>146</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:25:40 2024</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>121</v>
+      </c>
+      <c r="D147" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>147</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:25:50 2024</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>124</v>
+      </c>
+      <c r="D148" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:26:00 2024</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>123</v>
+      </c>
+      <c r="D149" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:26:10 2024</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>122</v>
+      </c>
+      <c r="D150" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:26:20 2024</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>123</v>
+      </c>
+      <c r="D151" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:26:30 2024</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>123</v>
+      </c>
+      <c r="D152" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:26:40 2024</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>123</v>
+      </c>
+      <c r="D153" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:26:50 2024</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>123</v>
+      </c>
+      <c r="D154" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>154</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:27:00 2024</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>123</v>
+      </c>
+      <c r="D155" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>155</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:27:10 2024</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>123</v>
+      </c>
+      <c r="D156" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>156</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:27:20 2024</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>122</v>
+      </c>
+      <c r="D157" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>157</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:27:30 2024</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>122</v>
+      </c>
+      <c r="D158" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>158</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:27:40 2024</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>121</v>
+      </c>
+      <c r="D159" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>159</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:27:50 2024</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>120</v>
+      </c>
+      <c r="D160" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>160</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:28:00 2024</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>119</v>
+      </c>
+      <c r="D161" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>161</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:28:10 2024</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>119</v>
+      </c>
+      <c r="D162" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>162</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:28:20 2024</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>121</v>
+      </c>
+      <c r="D163" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>163</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:28:30 2024</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>118</v>
+      </c>
+      <c r="D164" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>164</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:28:40 2024</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>118</v>
+      </c>
+      <c r="D165" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>165</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:28:50 2024</t>
+        </is>
+      </c>
+      <c r="C166" t="n">
+        <v>118</v>
+      </c>
+      <c r="D166" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>166</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:29:00 2024</t>
+        </is>
+      </c>
+      <c r="C167" t="n">
+        <v>117</v>
+      </c>
+      <c r="D167" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>167</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:29:10 2024</t>
+        </is>
+      </c>
+      <c r="C168" t="n">
+        <v>117</v>
+      </c>
+      <c r="D168" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>168</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:29:20 2024</t>
+        </is>
+      </c>
+      <c r="C169" t="n">
+        <v>117</v>
+      </c>
+      <c r="D169" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>169</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:29:30 2024</t>
+        </is>
+      </c>
+      <c r="C170" t="n">
+        <v>118</v>
+      </c>
+      <c r="D170" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>170</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:29:40 2024</t>
+        </is>
+      </c>
+      <c r="C171" t="n">
+        <v>117</v>
+      </c>
+      <c r="D171" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>171</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:29:50 2024</t>
+        </is>
+      </c>
+      <c r="C172" t="n">
+        <v>119</v>
+      </c>
+      <c r="D172" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>172</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:30:00 2024</t>
+        </is>
+      </c>
+      <c r="C173" t="n">
+        <v>118</v>
+      </c>
+      <c r="D173" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>173</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:30:10 2024</t>
+        </is>
+      </c>
+      <c r="C174" t="n">
+        <v>119</v>
+      </c>
+      <c r="D174" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>174</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:30:20 2024</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>120</v>
+      </c>
+      <c r="D175" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>175</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:30:42 2024</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>118</v>
+      </c>
+      <c r="D176" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>176</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:30:52 2024</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>118</v>
+      </c>
+      <c r="D177" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>177</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:31:18 2024</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
+        <v>119</v>
+      </c>
+      <c r="D178" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>178</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:45:16 2024</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>118</v>
+      </c>
+      <c r="D179" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>179</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:45:26 2024</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>118</v>
+      </c>
+      <c r="D180" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>180</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:45:36 2024</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
+        <v>117</v>
+      </c>
+      <c r="D181" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>181</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:45:46 2024</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>119</v>
+      </c>
+      <c r="D182" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>182</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:45:56 2024</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
+        <v>117</v>
+      </c>
+      <c r="D183" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>183</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:47:58 2024</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>117</v>
+      </c>
+      <c r="D184" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>184</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:01 2024</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>117</v>
+      </c>
+      <c r="D185" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>185</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:04 2024</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>117</v>
+      </c>
+      <c r="D186" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>186</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:07 2024</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
+        <v>117</v>
+      </c>
+      <c r="D187" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>187</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:10 2024</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>118</v>
+      </c>
+      <c r="D188" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>188</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:13 2024</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>117</v>
+      </c>
+      <c r="D189" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>189</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:16 2024</t>
+        </is>
+      </c>
+      <c r="C190" t="n">
+        <v>117</v>
+      </c>
+      <c r="D190" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>190</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:19 2024</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>117</v>
+      </c>
+      <c r="D191" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>191</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:22 2024</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
+        <v>163</v>
+      </c>
+      <c r="D192" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>192</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:25 2024</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>166</v>
+      </c>
+      <c r="D193" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>193</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:28 2024</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>172</v>
+      </c>
+      <c r="D194" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>194</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:31 2024</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>159</v>
+      </c>
+      <c r="D195" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>195</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:34 2024</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>150</v>
+      </c>
+      <c r="D196" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>196</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:37 2024</t>
+        </is>
+      </c>
+      <c r="C197" t="n">
+        <v>222</v>
+      </c>
+      <c r="D197" t="n">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>197</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:40 2024</t>
+        </is>
+      </c>
+      <c r="C198" t="n">
+        <v>291</v>
+      </c>
+      <c r="D198" t="n">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>198</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:43 2024</t>
+        </is>
+      </c>
+      <c r="C199" t="n">
+        <v>308</v>
+      </c>
+      <c r="D199" t="n">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>199</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:46 2024</t>
+        </is>
+      </c>
+      <c r="C200" t="n">
+        <v>287</v>
+      </c>
+      <c r="D200" t="n">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>200</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:49 2024</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>254</v>
+      </c>
+      <c r="D201" t="n">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>201</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:52 2024</t>
+        </is>
+      </c>
+      <c r="C202" t="n">
+        <v>273</v>
+      </c>
+      <c r="D202" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>202</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:55 2024</t>
+        </is>
+      </c>
+      <c r="C203" t="n">
+        <v>246</v>
+      </c>
+      <c r="D203" t="n">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>203</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:48:58 2024</t>
+        </is>
+      </c>
+      <c r="C204" t="n">
+        <v>215</v>
+      </c>
+      <c r="D204" t="n">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>204</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:01 2024</t>
+        </is>
+      </c>
+      <c r="C205" t="n">
+        <v>196</v>
+      </c>
+      <c r="D205" t="n">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>205</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:04 2024</t>
+        </is>
+      </c>
+      <c r="C206" t="n">
+        <v>186</v>
+      </c>
+      <c r="D206" t="n">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>206</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:07 2024</t>
+        </is>
+      </c>
+      <c r="C207" t="n">
+        <v>182</v>
+      </c>
+      <c r="D207" t="n">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>207</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:10 2024</t>
+        </is>
+      </c>
+      <c r="C208" t="n">
+        <v>176</v>
+      </c>
+      <c r="D208" t="n">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>208</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:13 2024</t>
+        </is>
+      </c>
+      <c r="C209" t="n">
+        <v>170</v>
+      </c>
+      <c r="D209" t="n">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>209</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:16 2024</t>
+        </is>
+      </c>
+      <c r="C210" t="n">
+        <v>166</v>
+      </c>
+      <c r="D210" t="n">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>210</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:19 2024</t>
+        </is>
+      </c>
+      <c r="C211" t="n">
+        <v>163</v>
+      </c>
+      <c r="D211" t="n">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>211</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:22 2024</t>
+        </is>
+      </c>
+      <c r="C212" t="n">
+        <v>161</v>
+      </c>
+      <c r="D212" t="n">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>212</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:25 2024</t>
+        </is>
+      </c>
+      <c r="C213" t="n">
+        <v>158</v>
+      </c>
+      <c r="D213" t="n">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>213</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:28 2024</t>
+        </is>
+      </c>
+      <c r="C214" t="n">
+        <v>155</v>
+      </c>
+      <c r="D214" t="n">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>214</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:31 2024</t>
+        </is>
+      </c>
+      <c r="C215" t="n">
+        <v>153</v>
+      </c>
+      <c r="D215" t="n">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>215</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:34 2024</t>
+        </is>
+      </c>
+      <c r="C216" t="n">
+        <v>151</v>
+      </c>
+      <c r="D216" t="n">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>216</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:37 2024</t>
+        </is>
+      </c>
+      <c r="C217" t="n">
+        <v>149</v>
+      </c>
+      <c r="D217" t="n">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>217</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:40 2024</t>
+        </is>
+      </c>
+      <c r="C218" t="n">
+        <v>148</v>
+      </c>
+      <c r="D218" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>218</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:43 2024</t>
+        </is>
+      </c>
+      <c r="C219" t="n">
+        <v>147</v>
+      </c>
+      <c r="D219" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>219</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:46 2024</t>
+        </is>
+      </c>
+      <c r="C220" t="n">
+        <v>145</v>
+      </c>
+      <c r="D220" t="n">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>220</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:49 2024</t>
+        </is>
+      </c>
+      <c r="C221" t="n">
+        <v>144</v>
+      </c>
+      <c r="D221" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>221</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:52 2024</t>
+        </is>
+      </c>
+      <c r="C222" t="n">
+        <v>143</v>
+      </c>
+      <c r="D222" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>222</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:55 2024</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>141</v>
+      </c>
+      <c r="D223" t="n">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>223</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:49:58 2024</t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>139</v>
+      </c>
+      <c r="D224" t="n">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>224</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:01 2024</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
+        <v>138</v>
+      </c>
+      <c r="D225" t="n">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>225</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:04 2024</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>137</v>
+      </c>
+      <c r="D226" t="n">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>226</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:07 2024</t>
+        </is>
+      </c>
+      <c r="C227" t="n">
+        <v>136</v>
+      </c>
+      <c r="D227" t="n">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>227</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:10 2024</t>
+        </is>
+      </c>
+      <c r="C228" t="n">
+        <v>135</v>
+      </c>
+      <c r="D228" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>228</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:13 2024</t>
+        </is>
+      </c>
+      <c r="C229" t="n">
+        <v>134</v>
+      </c>
+      <c r="D229" t="n">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>229</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:16 2024</t>
+        </is>
+      </c>
+      <c r="C230" t="n">
+        <v>135</v>
+      </c>
+      <c r="D230" t="n">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>230</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:19 2024</t>
+        </is>
+      </c>
+      <c r="C231" t="n">
+        <v>133</v>
+      </c>
+      <c r="D231" t="n">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>231</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:22 2024</t>
+        </is>
+      </c>
+      <c r="C232" t="n">
+        <v>132</v>
+      </c>
+      <c r="D232" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>232</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:25 2024</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>131</v>
+      </c>
+      <c r="D233" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>233</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:28 2024</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>132</v>
+      </c>
+      <c r="D234" t="n">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>234</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:31 2024</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
+        <v>131</v>
+      </c>
+      <c r="D235" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>235</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:34 2024</t>
+        </is>
+      </c>
+      <c r="C236" t="n">
+        <v>131</v>
+      </c>
+      <c r="D236" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>236</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:37 2024</t>
+        </is>
+      </c>
+      <c r="C237" t="n">
+        <v>132</v>
+      </c>
+      <c r="D237" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>237</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:40 2024</t>
+        </is>
+      </c>
+      <c r="C238" t="n">
+        <v>130</v>
+      </c>
+      <c r="D238" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>238</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:43 2024</t>
+        </is>
+      </c>
+      <c r="C239" t="n">
+        <v>129</v>
+      </c>
+      <c r="D239" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>239</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:46 2024</t>
+        </is>
+      </c>
+      <c r="C240" t="n">
+        <v>130</v>
+      </c>
+      <c r="D240" t="n">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>240</v>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:49 2024</t>
+        </is>
+      </c>
+      <c r="C241" t="n">
+        <v>130</v>
+      </c>
+      <c r="D241" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>241</v>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:52 2024</t>
+        </is>
+      </c>
+      <c r="C242" t="n">
+        <v>129</v>
+      </c>
+      <c r="D242" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>242</v>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:55 2024</t>
+        </is>
+      </c>
+      <c r="C243" t="n">
+        <v>128</v>
+      </c>
+      <c r="D243" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>243</v>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:50:58 2024</t>
+        </is>
+      </c>
+      <c r="C244" t="n">
+        <v>127</v>
+      </c>
+      <c r="D244" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>244</v>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:01 2024</t>
+        </is>
+      </c>
+      <c r="C245" t="n">
+        <v>126</v>
+      </c>
+      <c r="D245" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>245</v>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:04 2024</t>
+        </is>
+      </c>
+      <c r="C246" t="n">
+        <v>127</v>
+      </c>
+      <c r="D246" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>246</v>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:07 2024</t>
+        </is>
+      </c>
+      <c r="C247" t="n">
+        <v>127</v>
+      </c>
+      <c r="D247" t="n">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>247</v>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:10 2024</t>
+        </is>
+      </c>
+      <c r="C248" t="n">
+        <v>126</v>
+      </c>
+      <c r="D248" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>248</v>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:13 2024</t>
+        </is>
+      </c>
+      <c r="C249" t="n">
+        <v>125</v>
+      </c>
+      <c r="D249" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>249</v>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:16 2024</t>
+        </is>
+      </c>
+      <c r="C250" t="n">
+        <v>124</v>
+      </c>
+      <c r="D250" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>250</v>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:19 2024</t>
+        </is>
+      </c>
+      <c r="C251" t="n">
+        <v>124</v>
+      </c>
+      <c r="D251" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>251</v>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:22 2024</t>
+        </is>
+      </c>
+      <c r="C252" t="n">
+        <v>124</v>
+      </c>
+      <c r="D252" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>252</v>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:25 2024</t>
+        </is>
+      </c>
+      <c r="C253" t="n">
+        <v>124</v>
+      </c>
+      <c r="D253" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>253</v>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:28 2024</t>
+        </is>
+      </c>
+      <c r="C254" t="n">
+        <v>123</v>
+      </c>
+      <c r="D254" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>254</v>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:31 2024</t>
+        </is>
+      </c>
+      <c r="C255" t="n">
+        <v>173</v>
+      </c>
+      <c r="D255" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>255</v>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:34 2024</t>
+        </is>
+      </c>
+      <c r="C256" t="n">
+        <v>251</v>
+      </c>
+      <c r="D256" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>256</v>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:37 2024</t>
+        </is>
+      </c>
+      <c r="C257" t="n">
+        <v>234</v>
+      </c>
+      <c r="D257" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>257</v>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:40 2024</t>
+        </is>
+      </c>
+      <c r="C258" t="n">
+        <v>205</v>
+      </c>
+      <c r="D258" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>258</v>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:43 2024</t>
+        </is>
+      </c>
+      <c r="C259" t="n">
+        <v>184</v>
+      </c>
+      <c r="D259" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>259</v>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:46 2024</t>
+        </is>
+      </c>
+      <c r="C260" t="n">
+        <v>173</v>
+      </c>
+      <c r="D260" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>260</v>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:51:49 2024</t>
+        </is>
+      </c>
+      <c r="C261" t="n">
+        <v>165</v>
+      </c>
+      <c r="D261" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>261</v>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:02 2024</t>
+        </is>
+      </c>
+      <c r="C262" t="n">
+        <v>147</v>
+      </c>
+      <c r="D262" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>262</v>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:05 2024</t>
+        </is>
+      </c>
+      <c r="C263" t="n">
+        <v>145</v>
+      </c>
+      <c r="D263" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>263</v>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:08 2024</t>
+        </is>
+      </c>
+      <c r="C264" t="n">
+        <v>143</v>
+      </c>
+      <c r="D264" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>264</v>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:11 2024</t>
+        </is>
+      </c>
+      <c r="C265" t="n">
+        <v>140</v>
+      </c>
+      <c r="D265" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>265</v>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:14 2024</t>
+        </is>
+      </c>
+      <c r="C266" t="n">
+        <v>139</v>
+      </c>
+      <c r="D266" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>266</v>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:17 2024</t>
+        </is>
+      </c>
+      <c r="C267" t="n">
+        <v>137</v>
+      </c>
+      <c r="D267" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>267</v>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:20 2024</t>
+        </is>
+      </c>
+      <c r="C268" t="n">
+        <v>136</v>
+      </c>
+      <c r="D268" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>268</v>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:23 2024</t>
+        </is>
+      </c>
+      <c r="C269" t="n">
+        <v>135</v>
+      </c>
+      <c r="D269" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>269</v>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:26 2024</t>
+        </is>
+      </c>
+      <c r="C270" t="n">
+        <v>133</v>
+      </c>
+      <c r="D270" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>270</v>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:29 2024</t>
+        </is>
+      </c>
+      <c r="C271" t="n">
+        <v>133</v>
+      </c>
+      <c r="D271" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>271</v>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:32 2024</t>
+        </is>
+      </c>
+      <c r="C272" t="n">
+        <v>132</v>
+      </c>
+      <c r="D272" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>272</v>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:35 2024</t>
+        </is>
+      </c>
+      <c r="C273" t="n">
+        <v>132</v>
+      </c>
+      <c r="D273" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>273</v>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:38 2024</t>
+        </is>
+      </c>
+      <c r="C274" t="n">
+        <v>131</v>
+      </c>
+      <c r="D274" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>274</v>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:41 2024</t>
+        </is>
+      </c>
+      <c r="C275" t="n">
+        <v>130</v>
+      </c>
+      <c r="D275" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>275</v>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:44 2024</t>
+        </is>
+      </c>
+      <c r="C276" t="n">
+        <v>129</v>
+      </c>
+      <c r="D276" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>276</v>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:47 2024</t>
+        </is>
+      </c>
+      <c r="C277" t="n">
+        <v>130</v>
+      </c>
+      <c r="D277" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>277</v>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:50 2024</t>
+        </is>
+      </c>
+      <c r="C278" t="n">
+        <v>130</v>
+      </c>
+      <c r="D278" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>278</v>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:53 2024</t>
+        </is>
+      </c>
+      <c r="C279" t="n">
+        <v>129</v>
+      </c>
+      <c r="D279" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>279</v>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:56 2024</t>
+        </is>
+      </c>
+      <c r="C280" t="n">
+        <v>129</v>
+      </c>
+      <c r="D280" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>280</v>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:52:59 2024</t>
+        </is>
+      </c>
+      <c r="C281" t="n">
+        <v>128</v>
+      </c>
+      <c r="D281" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>281</v>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:02 2024</t>
+        </is>
+      </c>
+      <c r="C282" t="n">
+        <v>127</v>
+      </c>
+      <c r="D282" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>282</v>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:05 2024</t>
+        </is>
+      </c>
+      <c r="C283" t="n">
+        <v>126</v>
+      </c>
+      <c r="D283" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>283</v>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:08 2024</t>
+        </is>
+      </c>
+      <c r="C284" t="n">
+        <v>125</v>
+      </c>
+      <c r="D284" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>284</v>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:11 2024</t>
+        </is>
+      </c>
+      <c r="C285" t="n">
+        <v>124</v>
+      </c>
+      <c r="D285" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>285</v>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:14 2024</t>
+        </is>
+      </c>
+      <c r="C286" t="n">
+        <v>124</v>
+      </c>
+      <c r="D286" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>286</v>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:17 2024</t>
+        </is>
+      </c>
+      <c r="C287" t="n">
+        <v>124</v>
+      </c>
+      <c r="D287" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>287</v>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:20 2024</t>
+        </is>
+      </c>
+      <c r="C288" t="n">
+        <v>124</v>
+      </c>
+      <c r="D288" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>288</v>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:23 2024</t>
+        </is>
+      </c>
+      <c r="C289" t="n">
+        <v>123</v>
+      </c>
+      <c r="D289" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>289</v>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:26 2024</t>
+        </is>
+      </c>
+      <c r="C290" t="n">
+        <v>123</v>
+      </c>
+      <c r="D290" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>290</v>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:29 2024</t>
+        </is>
+      </c>
+      <c r="C291" t="n">
+        <v>122</v>
+      </c>
+      <c r="D291" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>291</v>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:32 2024</t>
+        </is>
+      </c>
+      <c r="C292" t="n">
+        <v>122</v>
+      </c>
+      <c r="D292" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>292</v>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:35 2024</t>
+        </is>
+      </c>
+      <c r="C293" t="n">
+        <v>122</v>
+      </c>
+      <c r="D293" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>293</v>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:38 2024</t>
+        </is>
+      </c>
+      <c r="C294" t="n">
+        <v>122</v>
+      </c>
+      <c r="D294" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>294</v>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:41 2024</t>
+        </is>
+      </c>
+      <c r="C295" t="n">
+        <v>121</v>
+      </c>
+      <c r="D295" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>295</v>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:44 2024</t>
+        </is>
+      </c>
+      <c r="C296" t="n">
+        <v>121</v>
+      </c>
+      <c r="D296" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>296</v>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:47 2024</t>
+        </is>
+      </c>
+      <c r="C297" t="n">
+        <v>121</v>
+      </c>
+      <c r="D297" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>297</v>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:50 2024</t>
+        </is>
+      </c>
+      <c r="C298" t="n">
+        <v>214</v>
+      </c>
+      <c r="D298" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>298</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:53 2024</t>
+        </is>
+      </c>
+      <c r="C299" t="n">
+        <v>246</v>
+      </c>
+      <c r="D299" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>299</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:56 2024</t>
+        </is>
+      </c>
+      <c r="C300" t="n">
+        <v>259</v>
+      </c>
+      <c r="D300" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>300</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:53:59 2024</t>
+        </is>
+      </c>
+      <c r="C301" t="n">
+        <v>237</v>
+      </c>
+      <c r="D301" t="n">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>301</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:02 2024</t>
+        </is>
+      </c>
+      <c r="C302" t="n">
+        <v>206</v>
+      </c>
+      <c r="D302" t="n">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>302</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:05 2024</t>
+        </is>
+      </c>
+      <c r="C303" t="n">
+        <v>189</v>
+      </c>
+      <c r="D303" t="n">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>303</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:08 2024</t>
+        </is>
+      </c>
+      <c r="C304" t="n">
+        <v>180</v>
+      </c>
+      <c r="D304" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>304</v>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:11 2024</t>
+        </is>
+      </c>
+      <c r="C305" t="n">
+        <v>171</v>
+      </c>
+      <c r="D305" t="n">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>305</v>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:14 2024</t>
+        </is>
+      </c>
+      <c r="C306" t="n">
+        <v>165</v>
+      </c>
+      <c r="D306" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>306</v>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:17 2024</t>
+        </is>
+      </c>
+      <c r="C307" t="n">
+        <v>161</v>
+      </c>
+      <c r="D307" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>307</v>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:20 2024</t>
+        </is>
+      </c>
+      <c r="C308" t="n">
+        <v>156</v>
+      </c>
+      <c r="D308" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>308</v>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:23 2024</t>
+        </is>
+      </c>
+      <c r="C309" t="n">
+        <v>159</v>
+      </c>
+      <c r="D309" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>309</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:26 2024</t>
+        </is>
+      </c>
+      <c r="C310" t="n">
+        <v>229</v>
+      </c>
+      <c r="D310" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>310</v>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:29 2024</t>
+        </is>
+      </c>
+      <c r="C311" t="n">
+        <v>260</v>
+      </c>
+      <c r="D311" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>311</v>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:32 2024</t>
+        </is>
+      </c>
+      <c r="C312" t="n">
+        <v>233</v>
+      </c>
+      <c r="D312" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>312</v>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:35 2024</t>
+        </is>
+      </c>
+      <c r="C313" t="n">
+        <v>224</v>
+      </c>
+      <c r="D313" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>313</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:38 2024</t>
+        </is>
+      </c>
+      <c r="C314" t="n">
+        <v>256</v>
+      </c>
+      <c r="D314" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>314</v>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:41 2024</t>
+        </is>
+      </c>
+      <c r="C315" t="n">
+        <v>255</v>
+      </c>
+      <c r="D315" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>315</v>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:44 2024</t>
+        </is>
+      </c>
+      <c r="C316" t="n">
+        <v>283</v>
+      </c>
+      <c r="D316" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>316</v>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:47 2024</t>
+        </is>
+      </c>
+      <c r="C317" t="n">
+        <v>278</v>
+      </c>
+      <c r="D317" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>317</v>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:50 2024</t>
+        </is>
+      </c>
+      <c r="C318" t="n">
+        <v>277</v>
+      </c>
+      <c r="D318" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>318</v>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:53 2024</t>
+        </is>
+      </c>
+      <c r="C319" t="n">
+        <v>276</v>
+      </c>
+      <c r="D319" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>319</v>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:56 2024</t>
+        </is>
+      </c>
+      <c r="C320" t="n">
+        <v>251</v>
+      </c>
+      <c r="D320" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>320</v>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:54:59 2024</t>
+        </is>
+      </c>
+      <c r="C321" t="n">
+        <v>221</v>
+      </c>
+      <c r="D321" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>321</v>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:02 2024</t>
+        </is>
+      </c>
+      <c r="C322" t="n">
+        <v>203</v>
+      </c>
+      <c r="D322" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>322</v>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:05 2024</t>
+        </is>
+      </c>
+      <c r="C323" t="n">
+        <v>191</v>
+      </c>
+      <c r="D323" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>323</v>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:08 2024</t>
+        </is>
+      </c>
+      <c r="C324" t="n">
+        <v>184</v>
+      </c>
+      <c r="D324" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>324</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:11 2024</t>
+        </is>
+      </c>
+      <c r="C325" t="n">
+        <v>177</v>
+      </c>
+      <c r="D325" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>325</v>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:14 2024</t>
+        </is>
+      </c>
+      <c r="C326" t="n">
+        <v>174</v>
+      </c>
+      <c r="D326" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>326</v>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:17 2024</t>
+        </is>
+      </c>
+      <c r="C327" t="n">
+        <v>169</v>
+      </c>
+      <c r="D327" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>327</v>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:20 2024</t>
+        </is>
+      </c>
+      <c r="C328" t="n">
+        <v>165</v>
+      </c>
+      <c r="D328" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>328</v>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:23 2024</t>
+        </is>
+      </c>
+      <c r="C329" t="n">
+        <v>162</v>
+      </c>
+      <c r="D329" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>329</v>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:26 2024</t>
+        </is>
+      </c>
+      <c r="C330" t="n">
+        <v>159</v>
+      </c>
+      <c r="D330" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>330</v>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:29 2024</t>
+        </is>
+      </c>
+      <c r="C331" t="n">
+        <v>156</v>
+      </c>
+      <c r="D331" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>331</v>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:32 2024</t>
+        </is>
+      </c>
+      <c r="C332" t="n">
+        <v>155</v>
+      </c>
+      <c r="D332" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>332</v>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:35 2024</t>
+        </is>
+      </c>
+      <c r="C333" t="n">
+        <v>153</v>
+      </c>
+      <c r="D333" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>333</v>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:38 2024</t>
+        </is>
+      </c>
+      <c r="C334" t="n">
+        <v>150</v>
+      </c>
+      <c r="D334" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>334</v>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:41 2024</t>
+        </is>
+      </c>
+      <c r="C335" t="n">
+        <v>149</v>
+      </c>
+      <c r="D335" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
+        <v>335</v>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:44 2024</t>
+        </is>
+      </c>
+      <c r="C336" t="n">
+        <v>147</v>
+      </c>
+      <c r="D336" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
+        <v>336</v>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:47 2024</t>
+        </is>
+      </c>
+      <c r="C337" t="n">
+        <v>145</v>
+      </c>
+      <c r="D337" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>337</v>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:50 2024</t>
+        </is>
+      </c>
+      <c r="C338" t="n">
+        <v>144</v>
+      </c>
+      <c r="D338" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>338</v>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:53 2024</t>
+        </is>
+      </c>
+      <c r="C339" t="n">
+        <v>142</v>
+      </c>
+      <c r="D339" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>339</v>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:56 2024</t>
+        </is>
+      </c>
+      <c r="C340" t="n">
+        <v>141</v>
+      </c>
+      <c r="D340" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>340</v>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:55:59 2024</t>
+        </is>
+      </c>
+      <c r="C341" t="n">
+        <v>140</v>
+      </c>
+      <c r="D341" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>341</v>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:56:02 2024</t>
+        </is>
+      </c>
+      <c r="C342" t="n">
+        <v>138</v>
+      </c>
+      <c r="D342" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>342</v>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:56:05 2024</t>
+        </is>
+      </c>
+      <c r="C343" t="n">
+        <v>138</v>
+      </c>
+      <c r="D343" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>343</v>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:56:08 2024</t>
+        </is>
+      </c>
+      <c r="C344" t="n">
+        <v>137</v>
+      </c>
+      <c r="D344" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>344</v>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:56:23 2024</t>
+        </is>
+      </c>
+      <c r="C345" t="n">
+        <v>134</v>
+      </c>
+      <c r="D345" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>345</v>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:56:26 2024</t>
+        </is>
+      </c>
+      <c r="C346" t="n">
+        <v>133</v>
+      </c>
+      <c r="D346" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
+        <v>346</v>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:56:29 2024</t>
+        </is>
+      </c>
+      <c r="C347" t="n">
+        <v>132</v>
+      </c>
+      <c r="D347" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
+        <v>347</v>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:56:32 2024</t>
+        </is>
+      </c>
+      <c r="C348" t="n">
+        <v>132</v>
+      </c>
+      <c r="D348" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="n">
+        <v>348</v>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:56:35 2024</t>
+        </is>
+      </c>
+      <c r="C349" t="n">
+        <v>131</v>
+      </c>
+      <c r="D349" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="n">
+        <v>349</v>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:56:38 2024</t>
+        </is>
+      </c>
+      <c r="C350" t="n">
+        <v>131</v>
+      </c>
+      <c r="D350" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="n">
+        <v>350</v>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:56:41 2024</t>
+        </is>
+      </c>
+      <c r="C351" t="n">
+        <v>131</v>
+      </c>
+      <c r="D351" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>351</v>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:56:44 2024</t>
+        </is>
+      </c>
+      <c r="C352" t="n">
+        <v>131</v>
+      </c>
+      <c r="D352" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
+        <v>352</v>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:56:47 2024</t>
+        </is>
+      </c>
+      <c r="C353" t="n">
+        <v>130</v>
+      </c>
+      <c r="D353" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="n">
+        <v>353</v>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:59:35 2024</t>
+        </is>
+      </c>
+      <c r="C354" t="n">
+        <v>119</v>
+      </c>
+      <c r="D354" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="n">
+        <v>354</v>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:59:38 2024</t>
+        </is>
+      </c>
+      <c r="C355" t="n">
+        <v>119</v>
+      </c>
+      <c r="D355" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="n">
+        <v>355</v>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:59:41 2024</t>
+        </is>
+      </c>
+      <c r="C356" t="n">
+        <v>119</v>
+      </c>
+      <c r="D356" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="n">
+        <v>356</v>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:59:44 2024</t>
+        </is>
+      </c>
+      <c r="C357" t="n">
+        <v>118</v>
+      </c>
+      <c r="D357" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="n">
+        <v>357</v>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:59:47 2024</t>
+        </is>
+      </c>
+      <c r="C358" t="n">
+        <v>118</v>
+      </c>
+      <c r="D358" t="n">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add new lawyer (model)
</commit_message>
<xml_diff>
--- a/lecturas_sensores.xlsx
+++ b/lecturas_sensores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D358"/>
+  <dimension ref="A1:D367"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6167,6 +6167,150 @@
         <v>128</v>
       </c>
     </row>
+    <row r="359">
+      <c r="A359" t="n">
+        <v>358</v>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:59:50 2024</t>
+        </is>
+      </c>
+      <c r="C359" t="n">
+        <v>118</v>
+      </c>
+      <c r="D359" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="n">
+        <v>359</v>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:59:53 2024</t>
+        </is>
+      </c>
+      <c r="C360" t="n">
+        <v>118</v>
+      </c>
+      <c r="D360" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="n">
+        <v>360</v>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:59:56 2024</t>
+        </is>
+      </c>
+      <c r="C361" t="n">
+        <v>118</v>
+      </c>
+      <c r="D361" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="n">
+        <v>361</v>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 01:59:59 2024</t>
+        </is>
+      </c>
+      <c r="C362" t="n">
+        <v>118</v>
+      </c>
+      <c r="D362" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="n">
+        <v>362</v>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 02:00:02 2024</t>
+        </is>
+      </c>
+      <c r="C363" t="n">
+        <v>118</v>
+      </c>
+      <c r="D363" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="n">
+        <v>363</v>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 02:00:05 2024</t>
+        </is>
+      </c>
+      <c r="C364" t="n">
+        <v>119</v>
+      </c>
+      <c r="D364" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="n">
+        <v>364</v>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 02:05:56 2024</t>
+        </is>
+      </c>
+      <c r="C365" t="n">
+        <v>116</v>
+      </c>
+      <c r="D365" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="n">
+        <v>365</v>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 02:05:59 2024</t>
+        </is>
+      </c>
+      <c r="C366" t="n">
+        <v>115</v>
+      </c>
+      <c r="D366" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="n">
+        <v>366</v>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Thu Oct 17 02:06:02 2024</t>
+        </is>
+      </c>
+      <c r="C367" t="n">
+        <v>115</v>
+      </c>
+      <c r="D367" t="n">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>